<commit_message>
all new examples rebased to most recent dev deleted onld branch
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/metadata_spleen_new_protocols.xlsx
+++ b/examples/spreadsheets/current/filled/metadata_spleen_new_protocols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/Dropbox/HCA/preview_release_new_protocol_format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/Dropbox (EBI)/HCA/preview_release_new_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E6461CF4-5B7D-C943-ADF9-B4E270D68705}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{801683F2-3069-C247-8F90-53BA926EE89F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="39580" windowHeight="20780" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25660" windowHeight="15660" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="489">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1517,51 +1517,6 @@
   </si>
   <si>
     <t>p1</t>
-  </si>
-  <si>
-    <t>enrichment_protocol.protocol_core.protocol_name</t>
-  </si>
-  <si>
-    <t>enrichment_protocol.protocol_core.protocol_description</t>
-  </si>
-  <si>
-    <t>enrichment_protocol.protocol_core.start_time</t>
-  </si>
-  <si>
-    <t>enrichment_protocol.process_core.protocol_location</t>
-  </si>
-  <si>
-    <t>enrichment_protocol.protocol_core.operator_identity</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.protocol_core.protocol_name</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.protocol_core.protocol_description</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.protocol_core.start_time</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.protocol_core.protocol_location</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.protocol_core.operator_identity</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.protocol_core.protocol_name</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.protocol_core.protocol_description</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.protocol_core.start_time</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.protocol_core.protocol_location</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.protocol_core.operator_identity</t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2125,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4178,8 +4133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4259,19 +4214,19 @@
         <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>270</v>
       </c>
       <c r="C4" t="s">
-        <v>490</v>
+        <v>271</v>
       </c>
       <c r="D4" t="s">
-        <v>491</v>
+        <v>272</v>
       </c>
       <c r="E4" t="s">
-        <v>492</v>
+        <v>273</v>
       </c>
       <c r="F4" t="s">
-        <v>493</v>
+        <v>274</v>
       </c>
       <c r="G4" t="s">
         <v>275</v>
@@ -4324,8 +4279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AO4" sqref="AO4"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4527,22 +4482,22 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>363</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>494</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>495</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>496</v>
+        <v>285</v>
       </c>
       <c r="E4" t="s">
-        <v>497</v>
+        <v>286</v>
       </c>
       <c r="F4" t="s">
-        <v>498</v>
+        <v>287</v>
       </c>
       <c r="G4" t="s">
         <v>288</v>
@@ -4702,8 +4657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4792,22 +4747,22 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>499</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s">
-        <v>500</v>
+        <v>323</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>324</v>
       </c>
       <c r="E4" t="s">
-        <v>502</v>
+        <v>325</v>
       </c>
       <c r="F4" t="s">
-        <v>503</v>
+        <v>326</v>
       </c>
       <c r="G4" t="s">
         <v>327</v>
@@ -4825,7 +4780,7 @@
         <v>331</v>
       </c>
       <c r="L4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="M4" t="s">
         <v>335</v>

</xml_diff>

<commit_message>
Updated ICA filled example spreadsheet.
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/metadata_spleen_new_protocols.xlsx
+++ b/examples/spreadsheets/current/filled/metadata_spleen_new_protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67FC19-BF8C-B94D-8E43-77D5387AC4EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CEAEF6-070D-1443-ABDA-271A9423FE3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="6920" windowWidth="26620" windowHeight="18780" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="28800" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -2630,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3685,7 +3685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>